<commit_message>
POT-1 fix View phe duyet the NT
</commit_message>
<xml_diff>
--- a/EPORTAL/obj/Release/Package/PackageTmp/App_Data/BM_Đăng ký thẻ người.xlsx
+++ b/EPORTAL/obj/Release/Package/PackageTmp/App_Data/BM_Đăng ký thẻ người.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thienld\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BaoBao\EPORTAL\EPORTAL\EPORTAL\App_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C669E022-B715-4CC1-8B89-05BC188E41FC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA36604C-2E5E-41C7-AC42-A10E431A46EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BM" sheetId="1" r:id="rId1"/>
@@ -30,9 +30,7 @@
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -41,34 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="121">
-  <si>
-    <r>
-      <t xml:space="preserve">BM.05/QT.20
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Ngày hiệu lực:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> 01/06/2023</t>
-    </r>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="57">
   <si>
     <t>ĐƠN ĐỀ NGHỊ CẤP LẠI/ GIA HẠN/ ĐIỀU CHỈNH THÔNG TIN THẺ NGƯỜI</t>
   </si>
@@ -111,9 +82,6 @@
     <t>Cổng đăng ký ra/vào</t>
   </si>
   <si>
-    <t>Nhóm nhà thầu</t>
-  </si>
-  <si>
     <t>Ghi chú</t>
   </si>
   <si>
@@ -147,222 +115,21 @@
     <t>2. HPDQ1 -  NHÀ MÁY LUYỆN CỐC</t>
   </si>
   <si>
-    <t>Phiên dịch</t>
-  </si>
-  <si>
-    <t>Nhóm 1.1</t>
-  </si>
-  <si>
     <t>3. HPDQ1 - NHÀ MÁY LUYỆN GANG</t>
   </si>
   <si>
     <t>Ca</t>
   </si>
   <si>
-    <t>HPDQ1 - NHÀ MÁY NGUYÊN LIỆU</t>
-  </si>
-  <si>
-    <t>Cổng 2 - HPDQ1</t>
-  </si>
-  <si>
-    <t>Khách chỉ vào làm việc tại văn phòng chính, văn phòng tạm, văn phòng bộ phận</t>
-  </si>
-  <si>
-    <t>Ban Giám đốc NT</t>
-  </si>
-  <si>
     <t>Hành chính (HC)</t>
   </si>
   <si>
-    <t>HPDQ1 -  NHÀ MÁY LUYỆN CỐC</t>
-  </si>
-  <si>
-    <t>Cổng 3 - HPDQ1</t>
-  </si>
-  <si>
-    <t>Nhóm 1.2</t>
-  </si>
-  <si>
-    <t>Nhà thầu làm việc tại VPC, VPT, VP bộ phận (trừ công việc xây dựng cơ bản)</t>
-  </si>
-  <si>
-    <t>Chỉ huy trưởng</t>
-  </si>
-  <si>
     <t>Ca ngày (CN)</t>
   </si>
   <si>
-    <t>HPDQ1 - NHÀ MÁY LUYỆN GANG</t>
-  </si>
-  <si>
-    <t>Cổng 4 - HPDQ1</t>
-  </si>
-  <si>
-    <t>Nhóm 2.1</t>
-  </si>
-  <si>
-    <t>Khách đi vào khu vực sản xuất</t>
-  </si>
-  <si>
-    <t>Chỉ huy phó</t>
-  </si>
-  <si>
     <t>Ca đêm (CĐ)</t>
   </si>
   <si>
-    <t>HPDQ1 - NHÀ MÁY NHIỆT ĐIỆN</t>
-  </si>
-  <si>
-    <t>Cổng 1 - HPDQ2</t>
-  </si>
-  <si>
-    <t>Nhóm 3.1</t>
-  </si>
-  <si>
-    <t>Giao nhận hàng hóa</t>
-  </si>
-  <si>
-    <t>Quản lý</t>
-  </si>
-  <si>
-    <t>HPDQ1 - NHÀ MÁY THIÊU KẾT VÊ VIÊN</t>
-  </si>
-  <si>
-    <t>Cổng 2 - HPDQ2</t>
-  </si>
-  <si>
-    <t>Nhóm 3.2</t>
-  </si>
-  <si>
-    <t>Nhà thầu làm việc từ 5 ngày trở lại (Không thực hiện công việc có yếu tố rủi ro cao)</t>
-  </si>
-  <si>
-    <t>Kỹ sư</t>
-  </si>
-  <si>
-    <t>HPDQ1 - NHÀ MÁY VÔI XI MĂNG</t>
-  </si>
-  <si>
-    <t>Cổng 3 (Hồ tân hòa) - HPDQ2</t>
-  </si>
-  <si>
-    <t>Nhóm 3.3</t>
-  </si>
-  <si>
-    <t>Nhà thầu làm việc từ 5 ngày trở lại (Thực hiện công việc có yếu tố rủi ro cao)</t>
-  </si>
-  <si>
-    <t>Nhân viên An toàn lao động</t>
-  </si>
-  <si>
-    <t>HPDQ1 -  KHU VỰC HỒ ĐIỀU HÒA</t>
-  </si>
-  <si>
-    <t>Cổng 4 (VPT) - HPDQ2</t>
-  </si>
-  <si>
-    <t>Nhóm 3.4</t>
-  </si>
-  <si>
-    <t>Nhà thầu làm việc từ trên 5 ngày</t>
-  </si>
-  <si>
-    <t>HPDQ1 - CỤM XỬ LÝ NƯỚC</t>
-  </si>
-  <si>
-    <t>Cổng 4 - HPDQ2</t>
-  </si>
-  <si>
-    <t>Nhóm 4.1</t>
-  </si>
-  <si>
-    <t>Chức vụ khác</t>
-  </si>
-  <si>
-    <t>HPDQ1 - NHÀ MÁY LUYỆN THÉP</t>
-  </si>
-  <si>
-    <t>Cổng 5 - HPDQ2</t>
-  </si>
-  <si>
-    <t>Nhóm 4.2</t>
-  </si>
-  <si>
-    <t>Nhà thầu làm việc từ 5 ngày trở lại</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HPDQ1 - NHÀ MÁY CÁN </t>
-  </si>
-  <si>
-    <t>Cổng 6 - HPDQ2</t>
-  </si>
-  <si>
-    <t>Nhóm 4.3</t>
-  </si>
-  <si>
-    <t>HPDQ2 - NHÀ MÁY CÁN</t>
-  </si>
-  <si>
-    <t>Cổng 7 - HPDQ2</t>
-  </si>
-  <si>
-    <t>HPDQ2 - NHÀ MÁY LUYỆN THÉP</t>
-  </si>
-  <si>
-    <t>Cổng Hải Quan - HPDQ2</t>
-  </si>
-  <si>
-    <t>HPDQ2 - CỤM XỬ LÝ NƯỚC TRUNG TÂM</t>
-  </si>
-  <si>
-    <t>Cổng 3 (phụ) - HPDQ1</t>
-  </si>
-  <si>
-    <t>HPDQ2 - NHÀ MÁY LUYỆN GANG</t>
-  </si>
-  <si>
-    <t>Cổng Cảng Tổng Hợp</t>
-  </si>
-  <si>
-    <t>HPDQ2 - NHÀ MÁY THIÊU KẾT VÊ VIÊN</t>
-  </si>
-  <si>
-    <t>Cổng 115ha - HPDQ2</t>
-  </si>
-  <si>
-    <t>HPDQ2 - NHÀ MÁY VÔI XI MĂNG</t>
-  </si>
-  <si>
-    <t>Cổng Hào Hưng - HPDQ1</t>
-  </si>
-  <si>
-    <t>HPDQ2 - NHÀ MÁY NHIỆT ĐIỆN</t>
-  </si>
-  <si>
-    <t>Cổng DQS - HPDQ1</t>
-  </si>
-  <si>
-    <t>HPDQ2 - NHÀ MÁY THIÊU KẾT VÊ VIÊN (LÒ XOAY ĐÁY)</t>
-  </si>
-  <si>
-    <t>Cổng Văn Phòng Chính</t>
-  </si>
-  <si>
-    <t>HPDQ2 - NHÀ MÁY LUYỆN CỐC</t>
-  </si>
-  <si>
-    <t>Cổng NM.CTCK</t>
-  </si>
-  <si>
-    <t>HPDQ2 - NHÀ MÁY NGUYÊN LIỆU</t>
-  </si>
-  <si>
-    <t>HPDQ2 - KHU VỰC DỰ CHỜ</t>
-  </si>
-  <si>
-    <t>Văn phòng chính</t>
-  </si>
-  <si>
     <t>Khu vực (chưa chốt dữ liệu)</t>
   </si>
   <si>
@@ -430,13 +197,31 @@
   </si>
   <si>
     <t>C</t>
+  </si>
+  <si>
+    <t>Điện thoại thông minh
+(Đánh dấu "X" nếu đăng ký)"</t>
+  </si>
+  <si>
+    <t>BM.03A/QT.20
+Ngày hiệu lực: 30/11/2024
+Lần sửa đổi: 02</t>
+  </si>
+  <si>
+    <t>CHỨC VỤ</t>
+  </si>
+  <si>
+    <t>KHU VỰC LÀM VIỆC</t>
+  </si>
+  <si>
+    <t>CỔNG ĐĂNG KÝ RA/VÀO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -487,14 +272,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <i/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
       <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -516,6 +293,20 @@
       <color rgb="FF495057"/>
       <name val="Segoe UI"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -625,7 +416,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -656,59 +447,69 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
@@ -727,23 +528,36 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -791,7 +605,7 @@
       <xdr:grpSpPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="2209800" cy="981075"/>
+          <a:ext cx="2210666" cy="975880"/>
           <a:chOff x="0" y="57150"/>
           <a:chExt cx="2219325" cy="981075"/>
         </a:xfrm>
@@ -1166,8 +980,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView topLeftCell="C1" zoomScale="55" zoomScaleNormal="55" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="Z44" sqref="Z44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.25" x14ac:dyDescent="0.25"/>
@@ -1186,7 +1000,7 @@
     <col min="13" max="14" width="10" style="9" customWidth="1"/>
     <col min="15" max="15" width="14.140625" style="9" customWidth="1"/>
     <col min="16" max="16" width="18.140625" style="10" customWidth="1"/>
-    <col min="17" max="17" width="83" style="9" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="83" style="10" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="37.5703125" style="9" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="20" style="9" customWidth="1"/>
     <col min="20" max="20" width="17.5703125" style="9" customWidth="1"/>
@@ -1196,363 +1010,366 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="1" customFormat="1" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K1" s="31" t="s">
+      <c r="C1" s="31"/>
+      <c r="K1" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
+      <c r="N1" s="35"/>
+      <c r="O1" s="35"/>
+      <c r="P1" s="35"/>
+      <c r="Q1" s="35"/>
+      <c r="R1" s="35"/>
+      <c r="S1" s="35"/>
+      <c r="T1" s="35"/>
+    </row>
+    <row r="2" spans="1:24" s="1" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
-      <c r="N1" s="31"/>
-      <c r="O1" s="31"/>
-      <c r="P1" s="31"/>
-      <c r="Q1" s="31"/>
-      <c r="R1" s="31"/>
-      <c r="S1" s="31"/>
-      <c r="T1" s="31"/>
-    </row>
-    <row r="2" spans="1:24" s="1" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="32" t="s">
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
+      <c r="K2" s="36"/>
+      <c r="L2" s="36"/>
+      <c r="M2" s="36"/>
+      <c r="N2" s="36"/>
+      <c r="O2" s="36"/>
+      <c r="P2" s="36"/>
+      <c r="Q2" s="36"/>
+      <c r="R2" s="36"/>
+      <c r="S2" s="36"/>
+      <c r="T2" s="36"/>
+    </row>
+    <row r="3" spans="1:24" s="1" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="32"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
+      <c r="K3" s="32"/>
+      <c r="L3" s="32"/>
+      <c r="M3" s="32"/>
+      <c r="N3" s="32"/>
+      <c r="O3" s="32"/>
+      <c r="P3" s="32"/>
+      <c r="Q3" s="32"/>
+      <c r="R3" s="32"/>
+      <c r="S3" s="32"/>
+      <c r="T3" s="32"/>
+    </row>
+    <row r="4" spans="1:24" s="1" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
-      <c r="M2" s="32"/>
-      <c r="N2" s="32"/>
-      <c r="O2" s="32"/>
-      <c r="P2" s="32"/>
-      <c r="Q2" s="32"/>
-      <c r="R2" s="32"/>
-      <c r="S2" s="32"/>
-      <c r="T2" s="32"/>
-    </row>
-    <row r="3" spans="1:24" s="1" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="42"/>
-      <c r="B3" s="42"/>
-      <c r="C3" s="42"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
-      <c r="I3" s="42"/>
-      <c r="J3" s="42"/>
-      <c r="K3" s="42"/>
-      <c r="L3" s="42"/>
-      <c r="M3" s="42"/>
-      <c r="N3" s="42"/>
-      <c r="O3" s="42"/>
-      <c r="P3" s="42"/>
-      <c r="Q3" s="42"/>
-      <c r="R3" s="42"/>
-      <c r="S3" s="42"/>
-      <c r="T3" s="42"/>
-    </row>
-    <row r="4" spans="1:24" s="1" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="33" t="s">
+      <c r="B4" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="33" t="s">
+      <c r="C4" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="35" t="s">
+      <c r="D4" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="35" t="s">
+      <c r="E4" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="35" t="s">
+      <c r="F4" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="35" t="s">
+      <c r="G4" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="35" t="s">
+      <c r="H4" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="39" t="s">
+      <c r="I4" s="34"/>
+      <c r="J4" s="34"/>
+      <c r="K4" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
-      <c r="K4" s="39" t="s">
+      <c r="L4" s="34"/>
+      <c r="M4" s="34"/>
+      <c r="N4" s="34"/>
+      <c r="O4" s="48"/>
+      <c r="P4" s="43" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q4" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="L4" s="40"/>
-      <c r="M4" s="40"/>
-      <c r="N4" s="40"/>
-      <c r="O4" s="41"/>
-      <c r="P4" s="35" t="s">
+      <c r="R4" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="Q4" s="37" t="s">
+      <c r="S4" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="R4" s="35" t="s">
+      <c r="T4" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="S4" s="35" t="s">
+      <c r="X4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="T4" s="33" t="s">
+    </row>
+    <row r="5" spans="1:24" s="1" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="38"/>
+      <c r="B5" s="38"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="X4" s="2" t="s">
+      <c r="I5" s="5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="1:24" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="34"/>
-      <c r="B5" s="34"/>
-      <c r="C5" s="36"/>
-      <c r="D5" s="36"/>
-      <c r="E5" s="36"/>
-      <c r="F5" s="36"/>
-      <c r="G5" s="36"/>
-      <c r="H5" s="5" t="s">
+      <c r="J5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="K5" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="J5" s="5" t="s">
+      <c r="L5" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="K5" s="5" t="s">
+      <c r="M5" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="L5" s="5" t="s">
+      <c r="N5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="M5" s="5" t="s">
+      <c r="O5" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="N5" s="5" t="s">
+      <c r="P5" s="44"/>
+      <c r="Q5" s="42"/>
+      <c r="R5" s="46"/>
+      <c r="S5" s="47"/>
+      <c r="T5" s="38"/>
+      <c r="X5" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="O5" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="P5" s="36"/>
-      <c r="Q5" s="38"/>
-      <c r="R5" s="36"/>
-      <c r="S5" s="36"/>
-      <c r="T5" s="34"/>
-      <c r="X5" s="4" t="s">
-        <v>25</v>
-      </c>
     </row>
     <row r="6" spans="1:24" s="7" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="19"/>
-      <c r="B6" s="22"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="22"/>
-      <c r="G6" s="23"/>
+      <c r="A6" s="18"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="22"/>
       <c r="H6" s="6"/>
-      <c r="I6" s="19"/>
-      <c r="J6" s="28"/>
-      <c r="K6" s="19"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="27"/>
+      <c r="K6" s="18"/>
       <c r="L6" s="6"/>
       <c r="M6" s="6"/>
-      <c r="N6" s="30"/>
+      <c r="N6" s="28"/>
       <c r="O6" s="6"/>
-      <c r="P6" s="20"/>
-      <c r="Q6" s="16"/>
+      <c r="P6" s="19"/>
+      <c r="Q6" s="30"/>
       <c r="R6" s="29"/>
-      <c r="S6" s="17"/>
+      <c r="S6" s="16"/>
       <c r="T6" s="6"/>
       <c r="X6" s="15"/>
     </row>
     <row r="7" spans="1:24" s="7" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="19"/>
-      <c r="B7" s="22"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="23"/>
+      <c r="A7" s="18"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="22"/>
       <c r="H7" s="6"/>
-      <c r="I7" s="19"/>
-      <c r="J7" s="28"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="27"/>
       <c r="K7" s="6"/>
-      <c r="L7" s="19"/>
+      <c r="L7" s="18"/>
       <c r="M7" s="6"/>
       <c r="N7" s="6"/>
       <c r="O7" s="6"/>
-      <c r="P7" s="20"/>
-      <c r="Q7" s="16"/>
+      <c r="P7" s="19"/>
+      <c r="Q7" s="30"/>
       <c r="R7" s="29"/>
-      <c r="S7" s="17"/>
+      <c r="S7" s="16"/>
       <c r="T7" s="6"/>
       <c r="X7" s="15"/>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A8" s="19"/>
-      <c r="B8" s="22"/>
-      <c r="C8" s="24"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="23"/>
+      <c r="A8" s="18"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="22"/>
       <c r="H8" s="6"/>
-      <c r="I8" s="19"/>
-      <c r="J8" s="28"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="27"/>
       <c r="K8" s="6"/>
-      <c r="L8" s="18"/>
-      <c r="M8" s="19"/>
+      <c r="L8" s="17"/>
+      <c r="M8" s="18"/>
       <c r="N8" s="6"/>
       <c r="O8" s="6"/>
-      <c r="P8" s="20"/>
-      <c r="Q8" s="16"/>
+      <c r="P8" s="19"/>
+      <c r="Q8" s="30"/>
       <c r="R8" s="29"/>
-      <c r="S8" s="17"/>
-      <c r="T8" s="18"/>
+      <c r="S8" s="16"/>
+      <c r="T8" s="17"/>
       <c r="X8" s="8"/>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A9" s="19"/>
-      <c r="B9" s="22"/>
-      <c r="C9" s="24"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="23"/>
+      <c r="A9" s="18"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="22"/>
       <c r="H9" s="6"/>
-      <c r="I9" s="19"/>
-      <c r="J9" s="28"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="27"/>
       <c r="K9" s="6"/>
-      <c r="L9" s="18"/>
+      <c r="L9" s="17"/>
       <c r="M9" s="6"/>
       <c r="N9" s="6"/>
       <c r="O9" s="6"/>
-      <c r="P9" s="20"/>
-      <c r="Q9" s="16"/>
+      <c r="P9" s="19"/>
+      <c r="Q9" s="30"/>
       <c r="R9" s="29"/>
-      <c r="S9" s="17"/>
-      <c r="T9" s="18"/>
+      <c r="S9" s="16"/>
+      <c r="T9" s="17"/>
       <c r="X9" s="8"/>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A10" s="19"/>
-      <c r="B10" s="22"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="26"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="23"/>
+      <c r="A10" s="18"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="22"/>
       <c r="H10" s="6"/>
-      <c r="I10" s="19"/>
-      <c r="J10" s="28"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="27"/>
       <c r="K10" s="6"/>
-      <c r="L10" s="18"/>
+      <c r="L10" s="17"/>
       <c r="M10" s="6"/>
-      <c r="N10" s="19"/>
+      <c r="N10" s="18"/>
       <c r="O10" s="6"/>
-      <c r="P10" s="20"/>
-      <c r="Q10" s="16"/>
+      <c r="P10" s="19"/>
+      <c r="Q10" s="30"/>
       <c r="R10" s="29"/>
-      <c r="S10" s="17"/>
+      <c r="S10" s="16"/>
       <c r="T10" s="6"/>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A11" s="19"/>
-      <c r="B11" s="22"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="23"/>
+      <c r="A11" s="18"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="21"/>
+      <c r="G11" s="22"/>
       <c r="H11" s="6"/>
-      <c r="I11" s="19"/>
-      <c r="J11" s="28"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="27"/>
       <c r="K11" s="6"/>
-      <c r="L11" s="18"/>
+      <c r="L11" s="17"/>
       <c r="M11" s="6"/>
       <c r="N11" s="6"/>
-      <c r="O11" s="19"/>
-      <c r="P11" s="20"/>
-      <c r="Q11" s="16"/>
+      <c r="O11" s="18"/>
+      <c r="P11" s="19"/>
+      <c r="Q11" s="30"/>
       <c r="R11" s="29"/>
-      <c r="S11" s="17"/>
+      <c r="S11" s="16"/>
       <c r="T11" s="6"/>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A12" s="19"/>
-      <c r="B12" s="22"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="23"/>
+      <c r="A12" s="18"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="22"/>
       <c r="H12" s="6"/>
-      <c r="I12" s="19"/>
-      <c r="J12" s="28"/>
+      <c r="I12" s="18"/>
+      <c r="J12" s="27"/>
       <c r="K12" s="6"/>
-      <c r="L12" s="18"/>
+      <c r="L12" s="17"/>
       <c r="M12" s="6"/>
-      <c r="N12" s="19"/>
+      <c r="N12" s="18"/>
       <c r="O12" s="6"/>
-      <c r="P12" s="20"/>
-      <c r="Q12" s="16"/>
+      <c r="P12" s="19"/>
+      <c r="Q12" s="30"/>
       <c r="R12" s="29"/>
-      <c r="S12" s="17"/>
-      <c r="T12" s="18"/>
+      <c r="S12" s="16"/>
+      <c r="T12" s="17"/>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A13" s="19"/>
-      <c r="B13" s="22"/>
-      <c r="C13" s="26"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="23"/>
+      <c r="A13" s="18"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="25"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="22"/>
       <c r="H13" s="6"/>
-      <c r="I13" s="19"/>
-      <c r="J13" s="28"/>
+      <c r="I13" s="18"/>
+      <c r="J13" s="27"/>
       <c r="K13" s="6"/>
-      <c r="L13" s="19"/>
-      <c r="M13" s="19"/>
+      <c r="L13" s="18"/>
+      <c r="M13" s="18"/>
       <c r="N13" s="6"/>
       <c r="O13" s="6"/>
-      <c r="P13" s="20"/>
-      <c r="Q13" s="16"/>
+      <c r="P13" s="19"/>
+      <c r="Q13" s="30"/>
       <c r="R13" s="29"/>
-      <c r="S13" s="17"/>
-      <c r="T13" s="18"/>
+      <c r="S13" s="16"/>
+      <c r="T13" s="17"/>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A14" s="19"/>
-      <c r="B14" s="22"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="21"/>
+      <c r="A14" s="18"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="20"/>
       <c r="H14" s="6"/>
-      <c r="I14" s="19"/>
-      <c r="J14" s="28"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="27"/>
       <c r="K14" s="6"/>
-      <c r="L14" s="19"/>
+      <c r="L14" s="18"/>
       <c r="M14" s="6"/>
       <c r="N14" s="6"/>
       <c r="O14" s="6"/>
-      <c r="P14" s="20"/>
-      <c r="Q14" s="16"/>
+      <c r="P14" s="19"/>
+      <c r="Q14" s="30"/>
       <c r="R14" s="29"/>
-      <c r="S14" s="17"/>
+      <c r="S14" s="16"/>
       <c r="T14" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="K4:O4"/>
+    <mergeCell ref="A3:T3"/>
     <mergeCell ref="H4:J4"/>
     <mergeCell ref="K1:T1"/>
     <mergeCell ref="A2:T2"/>
@@ -1568,12 +1385,10 @@
     <mergeCell ref="F4:F5"/>
     <mergeCell ref="G4:G5"/>
     <mergeCell ref="S4:S5"/>
-    <mergeCell ref="K4:O4"/>
-    <mergeCell ref="A3:T3"/>
   </mergeCells>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q1:Q2 Q4:Q5 Q15:Q1048576" xr:uid="{E7A21656-4460-4663-AA14-0834674789ED}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q1:Q2 Q15:Q1048576 R4:R5" xr:uid="{E7A21656-4460-4663-AA14-0834674789ED}">
       <formula1>$X$4:$X$9</formula1>
     </dataValidation>
   </dataValidations>
@@ -1585,10 +1400,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5FD10EF-70EC-4087-A1E1-0FF4CEC0B824}">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1602,331 +1417,181 @@
     <col min="10" max="10" width="22.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B1" s="14"/>
-      <c r="C1" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="D1" s="12"/>
-      <c r="E1" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="G1" s="11" t="s">
+      <c r="C1" s="49" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" s="50"/>
+      <c r="E1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" s="4"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="13"/>
+      <c r="G2" s="11"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="J1" s="11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="D2" s="12"/>
-      <c r="E2" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="G2" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="H2" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="J2" s="11" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
-        <v>40</v>
-      </c>
       <c r="B3" s="12"/>
-      <c r="C3" s="12" t="s">
-        <v>41</v>
-      </c>
+      <c r="C3" s="12"/>
       <c r="D3" s="12"/>
-      <c r="E3" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="G3" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="H3" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="J3" s="11" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E3" s="13"/>
+      <c r="G3" s="11"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="B4" s="12"/>
-      <c r="C4" s="12" t="s">
-        <v>47</v>
-      </c>
+      <c r="C4" s="12"/>
       <c r="D4" s="12"/>
-      <c r="E4" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="G4" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="H4" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="J4" s="11" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E4" s="13"/>
+      <c r="G4" s="11"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="12"/>
       <c r="B5" s="12"/>
-      <c r="C5" s="12" t="s">
-        <v>52</v>
-      </c>
+      <c r="C5" s="12"/>
       <c r="D5" s="12"/>
-      <c r="E5" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="H5" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="J5" s="11" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="E5" s="13"/>
+      <c r="G5" s="11"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="12"/>
       <c r="B6" s="12"/>
-      <c r="C6" s="12" t="s">
-        <v>57</v>
-      </c>
+      <c r="C6" s="12"/>
       <c r="D6" s="12"/>
-      <c r="E6" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="G6" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="H6" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="J6" s="11" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E6" s="13"/>
+      <c r="G6" s="11"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="12"/>
       <c r="B7" s="12"/>
-      <c r="C7" s="12" t="s">
-        <v>62</v>
-      </c>
+      <c r="C7" s="12"/>
       <c r="D7" s="12"/>
-      <c r="E7" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="G7" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="H7" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="J7" s="11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E7" s="13"/>
+      <c r="G7" s="11"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="12"/>
       <c r="B8" s="12"/>
-      <c r="C8" s="12" t="s">
-        <v>66</v>
-      </c>
+      <c r="C8" s="12"/>
       <c r="D8" s="12"/>
-      <c r="E8" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="G8" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="H8" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="J8" s="11" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E8" s="13"/>
+      <c r="G8" s="11"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="12"/>
       <c r="B9" s="12"/>
-      <c r="C9" s="12" t="s">
-        <v>70</v>
-      </c>
+      <c r="C9" s="12"/>
       <c r="D9" s="12"/>
-      <c r="E9" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="G9" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="H9" s="11" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E9" s="13"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="12"/>
       <c r="B10" s="12"/>
-      <c r="C10" s="12" t="s">
-        <v>74</v>
-      </c>
+      <c r="C10" s="12"/>
       <c r="D10" s="12"/>
-      <c r="E10" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="G10" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="H10" s="11" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E10" s="13"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="12"/>
       <c r="B11" s="12"/>
-      <c r="C11" s="12" t="s">
-        <v>77</v>
-      </c>
+      <c r="C11" s="12"/>
       <c r="D11" s="12"/>
-      <c r="E11" s="13" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E11" s="13"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="12"/>
       <c r="B12" s="12"/>
-      <c r="C12" s="12" t="s">
-        <v>79</v>
-      </c>
+      <c r="C12" s="12"/>
       <c r="D12" s="12"/>
-      <c r="E12" s="13" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E12" s="13"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="12"/>
-      <c r="C13" s="12" t="s">
-        <v>81</v>
-      </c>
+      <c r="C13" s="12"/>
       <c r="D13" s="12"/>
-      <c r="E13" s="13" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E13" s="13"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="12"/>
       <c r="B14" s="12"/>
-      <c r="C14" s="12" t="s">
-        <v>83</v>
-      </c>
+      <c r="C14" s="12"/>
       <c r="D14" s="12"/>
-      <c r="E14" s="13" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E14" s="13"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="12"/>
       <c r="B15" s="12"/>
-      <c r="C15" s="12" t="s">
-        <v>85</v>
-      </c>
+      <c r="C15" s="12"/>
       <c r="D15" s="12"/>
-      <c r="E15" s="13" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E15" s="13"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="12"/>
       <c r="B16" s="12"/>
-      <c r="C16" s="12" t="s">
-        <v>87</v>
-      </c>
+      <c r="C16" s="12"/>
       <c r="D16" s="12"/>
-      <c r="E16" s="13" t="s">
-        <v>88</v>
-      </c>
+      <c r="E16" s="13"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="12"/>
       <c r="B17" s="12"/>
-      <c r="C17" s="12" t="s">
-        <v>89</v>
-      </c>
+      <c r="C17" s="12"/>
       <c r="D17" s="12"/>
-      <c r="E17" s="13" t="s">
-        <v>90</v>
-      </c>
+      <c r="E17" s="13"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="12"/>
       <c r="B18" s="12"/>
-      <c r="C18" s="12" t="s">
-        <v>91</v>
-      </c>
+      <c r="C18" s="12"/>
       <c r="D18" s="12"/>
-      <c r="E18" s="13" t="s">
-        <v>92</v>
-      </c>
+      <c r="E18" s="13"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="12"/>
       <c r="B19" s="12"/>
-      <c r="C19" s="12" t="s">
-        <v>93</v>
-      </c>
+      <c r="C19" s="12"/>
       <c r="D19" s="12"/>
-      <c r="E19" s="13" t="s">
-        <v>94</v>
-      </c>
+      <c r="E19" s="13"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="12"/>
       <c r="B20" s="12"/>
-      <c r="C20" s="12" t="s">
-        <v>95</v>
-      </c>
+      <c r="C20" s="12"/>
       <c r="D20" s="12"/>
       <c r="E20" s="13"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="12"/>
       <c r="B21" s="12"/>
-      <c r="C21" s="12" t="s">
-        <v>96</v>
-      </c>
+      <c r="C21" s="12"/>
       <c r="D21" s="12"/>
       <c r="E21" s="12"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="12"/>
       <c r="B22" s="12"/>
-      <c r="C22" s="12" t="s">
-        <v>97</v>
-      </c>
+      <c r="C22" s="12"/>
       <c r="D22" s="12"/>
       <c r="E22" s="12"/>
     </row>
@@ -1957,144 +1622,144 @@
   <sheetData>
     <row r="1" spans="1:2" s="3" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
-        <v>99</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
-        <v>100</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
-        <v>101</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
-        <v>102</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
-        <v>103</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
-        <v>104</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
-        <v>105</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
-        <v>106</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="s">
-        <v>107</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B14" s="4" t="s">
-        <v>108</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
-        <v>109</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="s">
-        <v>110</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="s">
-        <v>111</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" s="4" t="s">
-        <v>112</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" s="4" t="s">
-        <v>113</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" s="4" t="s">
-        <v>114</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
-        <v>115</v>
+        <v>46</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22" s="4" t="s">
-        <v>116</v>
+        <v>47</v>
       </c>
     </row>
     <row r="581" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A581" s="4" t="s">
-        <v>117</v>
+        <v>48</v>
       </c>
     </row>
     <row r="582" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A582" s="4" t="s">
-        <v>118</v>
+        <v>49</v>
       </c>
     </row>
     <row r="583" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A583" s="4" t="s">
-        <v>119</v>
+        <v>50</v>
       </c>
     </row>
     <row r="584" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A584" s="4" t="s">
-        <v>120</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>